<commit_message>
Update experiment and results.
</commit_message>
<xml_diff>
--- a/results/results_weights_mse_optim.xlsx
+++ b/results/results_weights_mse_optim.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mateu\CLionProjects\knn_ensemble_research\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{784C39AE-5F2F-4E5B-BAF9-1120EF110A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADF64A55-336F-418A-8655-BFB92B962927}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{AF0712F2-2DE8-4AC9-8CB8-C23D62550FE6}"/>
   </bookViews>
   <sheets>
     <sheet name="Multiplying by individual accs" sheetId="1" r:id="rId1"/>
+    <sheet name="Without accs mult" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="81">
   <si>
     <t>Accuracy</t>
   </si>
@@ -217,13 +218,64 @@
   </si>
   <si>
     <t xml:space="preserve"> [0.126, 0.000, 0.256, 0.275, 0.174, 0.016, 0.153]</t>
+  </si>
+  <si>
+    <t>[0.666, 0.545, 0.688, 0.582, 0.689, 0.581, 0.688]</t>
+  </si>
+  <si>
+    <t>[0.687, 0.529, 0.689, 0.582, 0.706, 0.584, 0.693]</t>
+  </si>
+  <si>
+    <t>[0.166, 0.000, 0.104, 0.089, 0.194, 0.171, 0.276]</t>
+  </si>
+  <si>
+    <t>MSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.500, 0.500, 0.500, 0.500, 0.500, 0.500, 0.500]</t>
+  </si>
+  <si>
+    <t>[0.000, 0.039, 0.072, 0.006, 0.000, 0.000, 0.882]</t>
+  </si>
+  <si>
+    <t>[0.253, 0.070, 0.183, 0.142, 0.163, 0.000, 0.190]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.000, 0.000, 0.181, 0.000, 0.213, 0.027, 0.579]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.926, 0.598, 0.927, 0.363, 0.945, 0.377, 0.952]</t>
+  </si>
+  <si>
+    <t>[0.925, 0.607, 0.924, 0.363, 0.940, 0.378, 0.950]</t>
+  </si>
+  <si>
+    <t>[0.204, 0.029, 0.176, 0.290, 0.095, 0.000, 0.206]</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> [0.654, 0.252, 0.674, 0.257, 0.635, 0.254, 0.675]</t>
+  </si>
+  <si>
+    <t>[0.126, 0.000, 0.256, 0.275, 0.174, 0.016, 0.153]</t>
+  </si>
+  <si>
+    <t>[0.754, 0.637, 0.713, 0.636, 0.605, 0.626, 0.839]</t>
+  </si>
+  <si>
+    <t>[0.927, 0.933, 0.928, 0.928, 0.933, 0.933, 0.928]</t>
+  </si>
+  <si>
+    <t>[0.930, 0.933, 0.931, 0.931, 0.933, 0.933, 0.929]</t>
+  </si>
+  <si>
+    <t>[0.918, 0.933, 0.918, 0.912, 0.933, 0.933, 0.920]</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -244,14 +296,6 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Liberation Sans"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -298,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -322,13 +366,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -648,7 +697,7 @@
   <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -662,21 +711,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="16" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="F1" s="11" t="s">
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="F1" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="11" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -950,12 +999,12 @@
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="11" t="s">
+      <c r="A15" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="B15" s="11"/>
-      <c r="C15" s="11"/>
-      <c r="D15" s="11"/>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="2" t="s">
@@ -978,7 +1027,7 @@
       <c r="B17" s="7">
         <v>62936</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>31</v>
       </c>
       <c r="D17" s="2" t="s">
@@ -1108,4 +1157,583 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7354AEC3-AE75-4FC4-90B9-15C084664997}">
+  <dimension ref="A1:K26"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="22" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="41.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="F1" s="16" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+    </row>
+    <row r="2" spans="1:11">
+      <c r="A2" s="11" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
+      <c r="A3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" s="7">
+        <v>67957</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="6">
+        <v>93750</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="H3" s="6">
+        <v>78213</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="K3" s="6">
+        <v>66500</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" s="15">
+        <v>82616</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" s="6">
+        <v>492918</v>
+      </c>
+      <c r="G4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="H4" s="6">
+        <v>83687</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="K4" s="14">
+        <v>492918</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="7">
+        <v>65519</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="6">
+        <v>298170</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H5" s="7">
+        <v>68281</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="K5" s="6">
+        <v>269118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="A6" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="5"/>
+      <c r="G6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+      <c r="K6" s="5"/>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="7">
+        <v>90111</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E7" s="6">
+        <v>101808</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="6">
+        <v>89583</v>
+      </c>
+      <c r="I7" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" s="6">
+        <v>125878</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="A8" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="9">
+        <v>72439</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="E8" s="13">
+        <v>565572</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H8" s="10">
+        <v>73936</v>
+      </c>
+      <c r="I8" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K8" s="6">
+        <v>516713</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="A9" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="7">
+        <v>88681</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E9" s="6">
+        <v>176000</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="H9" s="6">
+        <v>92534</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="K9" s="6">
+        <v>157750</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
+      <c r="A10" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="9">
+        <v>81460</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="6">
+        <v>105115</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="H10" s="10">
+        <v>76968</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="K10" s="6">
+        <v>126718</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B11" s="7">
+        <v>47346</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" s="6">
+        <v>611755</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H11" s="7">
+        <v>47359</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K11" s="6">
+        <v>588807</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
+      <c r="A12" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="7">
+        <v>95193</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="6">
+        <v>70160</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H12" s="10">
+        <v>95456</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="K12" s="6">
+        <v>71276</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="1"/>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="A15" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="A16" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="7">
+        <v>62936</v>
+      </c>
+      <c r="C17" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="6">
+        <v>69000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="7">
+        <v>83516</v>
+      </c>
+      <c r="C18" t="s">
+        <v>53</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E18" s="6">
+        <v>484681</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" s="7">
+        <v>67314</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="E19" s="6">
+        <v>275390</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="5"/>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="7">
+        <v>89583</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E21" s="6">
+        <v>110933</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="9">
+        <v>72439</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E22" s="6">
+        <v>540784</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="7">
+        <v>91686</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="E23" s="6">
+        <v>160000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="9">
+        <v>81325</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E24" s="6">
+        <v>107802</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="13">
+        <v>46242</v>
+      </c>
+      <c r="C25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" t="s">
+        <v>75</v>
+      </c>
+      <c r="E25" s="13">
+        <v>603887</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="9">
+        <v>95243</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="E26" s="6">
+        <v>69894</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="A15:D15"/>
+  </mergeCells>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>